<commit_message>
Modificacion CRG Facturados para omitir INC y Automatizacion Reporte Sigehos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/tipo_financiador.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/tipo_financiador.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$B$1021</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$B$1069</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="1028">
   <si>
     <t xml:space="preserve">Financiador</t>
   </si>
@@ -3038,6 +3038,75 @@
   </si>
   <si>
     <t xml:space="preserve">- CAJA DE PREV. SOCIAL DE PROF. DE ING. DE SANTA FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRINIDAD - SANATORIO DE LA TRINIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- SECRETARIA DE DESARROLLO SOCIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- SECRETARIA DE DESARROLLO SOCIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCLUIR SALUD CORDOBA - INCLUIR SALUD CORDOBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELEGACION METR - DELEGACION METROPOLITANA S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCLUIR SALUD CHUBUT - INCLUIR SALUD CHUBUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIEMPOMEDICO - TIEMPO MEDICO S.R.L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- UNIDAD DE GESTIO OPERATIVA FERROVIARIA DE EMERGENC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDICINA ESENCI - MEDICINA ESENCIAL S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCLUIR OTROS - INCLUIR SALUD OTROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMPSI - ASOCIACION MUTUAL DE PSICOLOGOS AMPSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREMEDIC - GRUPO PREMEDIC S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINIST.SALUD SA - MINISTERIO DE SALUD PUBLICA DEL GOBIERNO DE LA PROVINCIA DE SALTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERCANTIL ANDIN - COMPAÃ‘ÃA DE SEGUROS LA MERCANTIL ANDINA S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSUL.BOLIVIA - CONSULADO GENERAL DE BOLIVIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS PORTUARIOS P - OBRA SOCIAL PORTUARIOS DE PUERTO SAN MARTIN Y BELLA VISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBRA SOCIAL DE DIRECCION WITCE - OBRA SOCIAL DE DIRECCION WITCEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCHCAPE SHIPPI - INCHCAPE SHIPPING SERVICES ARGENTINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCIA SALUD HTAL - PROVINCIA SALUD HOSPITAL FRANCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSUL.UCRANIA - CONSULADO GENERAL DE UCRANIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUZ ART SA - LUZ ART SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSPAISM - OBRA SOCIAL DEL PERSONAL DEL AZUCAR INGENIO SAN MARTIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERCANTIL ANDIN - COMPAÑÍA DE SEGUROS LA MERCANTIL ANDINA S.A.</t>
   </si>
 </sst>
 </file>
@@ -3087,7 +3156,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3098,6 +3167,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9B8B8"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -3137,7 +3212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3158,6 +3233,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3167,11 +3246,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB9B8B8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3263,13 +3349,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1039"/>
+  <dimension ref="A1:B1069"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1014" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1043" activeCellId="0" sqref="A1043"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="145.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.71"/>
@@ -11587,8 +11673,248 @@
         <v>5</v>
       </c>
     </row>
+    <row r="1040" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1040" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1040" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1041" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1041" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B1041" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1042" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1042" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1042" s="0" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="1043" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1043" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1043" s="0" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="1044" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1044" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B1044" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1045" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1045" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1045" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1046" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1046" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1046" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1047" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1047" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1047" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1048" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1048" s="0" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1048" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1049" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1049" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1049" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1050" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1050" s="5" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1050" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1051" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1051" s="0" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1051" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1052" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1052" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1053" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1053" s="0" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1053" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1054" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1054" s="0" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1054" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1055" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1055" s="0" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1055" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1056" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1056" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1056" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1057" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1057" s="0" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1057" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1058" s="0" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B1058" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1059" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1059" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1059" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1060" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1060" s="0" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B1060" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1061" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1061" s="0" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1061" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1062" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1062" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1062" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1063" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1063" s="0" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B1063" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1064" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1064" s="0" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B1064" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1065" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1065" s="0" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B1065" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1066" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1066" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1067" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1067" s="0" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1067" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1068" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1068" s="0" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1068" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1069" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1069" s="0" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1069" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B1021"/>
+  <autoFilter ref="A1:B1069"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>